<commit_message>
completed all threshold outputs
</commit_message>
<xml_diff>
--- a/outputs/fft-p__Firmicutes_A.xlsx
+++ b/outputs/fft-p__Firmicutes_A.xlsx
@@ -45550,7 +45550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45594,6 +45594,11 @@
           <t>rejection-0.98</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -45628,6 +45633,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -45662,6 +45672,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -45696,6 +45711,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -45730,6 +45750,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -45764,6 +45789,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -45798,6 +45828,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -45832,6 +45867,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -45866,6 +45906,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -45900,6 +45945,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -45934,6 +45984,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -45968,6 +46023,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -46002,6 +46062,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -46036,6 +46101,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -46070,6 +46140,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -46104,6 +46179,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -46138,6 +46218,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -46172,6 +46257,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -46206,6 +46296,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
@@ -46240,6 +46335,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
@@ -46274,6 +46374,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
@@ -46308,6 +46413,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
@@ -46342,6 +46452,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
@@ -46376,6 +46491,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
@@ -46410,6 +46530,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
@@ -46444,6 +46569,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
@@ -46478,6 +46608,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
@@ -46512,6 +46647,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
@@ -46546,6 +46686,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
@@ -46580,6 +46725,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
@@ -46614,6 +46764,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
@@ -46648,6 +46803,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
@@ -46682,6 +46842,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
@@ -46716,6 +46881,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
@@ -46750,6 +46920,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
@@ -46784,6 +46959,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
@@ -46818,6 +46998,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
@@ -46852,6 +47037,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
@@ -46886,6 +47076,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
@@ -46920,6 +47115,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
@@ -46954,6 +47154,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
@@ -46988,6 +47193,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
@@ -47022,6 +47232,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
@@ -47056,6 +47271,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
@@ -47090,6 +47310,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
@@ -47124,6 +47349,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
@@ -47158,6 +47388,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
@@ -47192,6 +47427,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
@@ -47226,6 +47466,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
@@ -47260,6 +47505,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
@@ -47294,6 +47544,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
@@ -47328,6 +47583,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
@@ -47362,6 +47622,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="6" t="inlineStr">
@@ -47396,6 +47661,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
@@ -47430,6 +47700,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
@@ -47464,6 +47739,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
@@ -47498,6 +47778,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
@@ -47532,6 +47817,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
@@ -47562,6 +47852,11 @@
         </is>
       </c>
       <c r="H59" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
         <is>
           <t>c__Clostridia</t>
         </is>
@@ -47578,7 +47873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47622,6 +47917,11 @@
           <t>rejection-0.98</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -47656,6 +47956,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -47690,6 +47995,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -47724,6 +48034,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -47758,6 +48073,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -47792,6 +48112,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -47826,6 +48151,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -47860,6 +48190,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -47894,6 +48229,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -47928,6 +48268,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -47962,6 +48307,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -47996,6 +48346,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -48030,6 +48385,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -48064,6 +48424,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -48098,6 +48463,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -48132,6 +48502,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -48166,6 +48541,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -48200,6 +48580,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -48234,6 +48619,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
@@ -48268,6 +48658,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
@@ -48302,6 +48697,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
@@ -48336,6 +48736,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
@@ -48370,6 +48775,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
@@ -48404,6 +48814,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
@@ -48438,6 +48853,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
@@ -48472,6 +48892,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
@@ -48506,6 +48931,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
@@ -48540,6 +48970,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
@@ -48574,6 +49009,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
@@ -48608,6 +49048,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
@@ -48642,6 +49087,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
@@ -48676,6 +49126,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
@@ -48710,6 +49165,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
@@ -48744,6 +49204,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
@@ -48778,6 +49243,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
@@ -48812,6 +49282,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
@@ -48846,6 +49321,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
@@ -48880,6 +49360,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
@@ -48914,6 +49399,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
@@ -48948,6 +49438,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
@@ -48982,6 +49477,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
@@ -49016,6 +49516,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
@@ -49050,6 +49555,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
@@ -49084,6 +49594,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
@@ -49118,6 +49633,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
@@ -49152,6 +49672,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
@@ -49186,6 +49711,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
@@ -49220,6 +49750,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
@@ -49254,6 +49789,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
@@ -49288,6 +49828,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
@@ -49322,6 +49867,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
@@ -49356,6 +49906,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
@@ -49386,6 +49941,11 @@
         </is>
       </c>
       <c r="H53" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
         <is>
           <t>reject</t>
         </is>
@@ -49402,7 +49962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49446,6 +50006,11 @@
           <t>rejection-0.98</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -49480,6 +50045,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -49514,6 +50084,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -49548,6 +50123,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -49582,6 +50162,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -49616,6 +50201,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -49650,6 +50240,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -49684,6 +50279,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -49718,6 +50318,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -49752,6 +50357,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -49786,6 +50396,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -49820,6 +50435,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -49854,6 +50474,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -49888,6 +50513,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -49922,6 +50552,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -49956,6 +50591,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -49990,6 +50630,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -50024,6 +50669,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -50058,6 +50708,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
@@ -50092,6 +50747,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
@@ -50126,6 +50786,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
@@ -50160,6 +50825,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
@@ -50194,6 +50864,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
@@ -50228,6 +50903,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
@@ -50262,6 +50942,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
@@ -50296,6 +50981,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
@@ -50330,6 +51020,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
@@ -50364,6 +51059,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
@@ -50398,6 +51098,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
@@ -50432,6 +51137,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
@@ -50466,6 +51176,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
@@ -50500,6 +51215,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
@@ -50534,6 +51254,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
@@ -50568,6 +51293,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
@@ -50602,6 +51332,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
@@ -50636,6 +51371,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
@@ -50670,6 +51410,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
@@ -50704,6 +51449,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
@@ -50738,6 +51488,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
@@ -50772,6 +51527,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
@@ -50806,6 +51566,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
@@ -50840,6 +51605,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
@@ -50874,6 +51644,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
@@ -50908,6 +51683,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
@@ -50942,6 +51722,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
@@ -50976,6 +51761,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
@@ -51010,6 +51800,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
@@ -51044,6 +51839,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
@@ -51078,6 +51878,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
@@ -51112,6 +51917,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
@@ -51146,6 +51956,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
@@ -51180,6 +51995,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
@@ -51214,6 +52034,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="6" t="inlineStr">
@@ -51248,6 +52073,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
@@ -51282,6 +52112,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
@@ -51316,6 +52151,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
@@ -51350,6 +52190,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
@@ -51384,6 +52229,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
@@ -51418,6 +52268,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
@@ -51452,6 +52307,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
@@ -51486,6 +52346,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="6" t="inlineStr">
@@ -51520,6 +52385,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="6" t="inlineStr">
@@ -51554,6 +52424,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
@@ -51588,6 +52463,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
@@ -51622,6 +52502,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="6" t="inlineStr">
@@ -51656,6 +52541,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="6" t="inlineStr">
@@ -51690,6 +52580,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="6" t="inlineStr">
@@ -51724,6 +52619,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
@@ -51758,6 +52658,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="6" t="inlineStr">
@@ -51792,6 +52697,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="6" t="inlineStr">
@@ -51826,6 +52736,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="6" t="inlineStr">
@@ -51860,6 +52775,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="6" t="inlineStr">
@@ -51894,6 +52814,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="6" t="inlineStr">
@@ -51928,6 +52853,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="6" t="inlineStr">
@@ -51962,6 +52892,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="6" t="inlineStr">
@@ -51996,6 +52931,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="6" t="inlineStr">
@@ -52030,6 +52970,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="6" t="inlineStr">
@@ -52064,6 +53009,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="6" t="inlineStr">
@@ -52098,6 +53048,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="6" t="inlineStr">
@@ -52132,6 +53087,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="6" t="inlineStr">
@@ -52166,6 +53126,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="6" t="inlineStr">
@@ -52200,6 +53165,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="6" t="inlineStr">
@@ -52234,6 +53204,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="6" t="inlineStr">
@@ -52268,6 +53243,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="6" t="inlineStr">
@@ -52302,6 +53282,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="6" t="inlineStr">
@@ -52336,6 +53321,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="6" t="inlineStr">
@@ -52370,6 +53360,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="6" t="inlineStr">
@@ -52404,6 +53399,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="6" t="inlineStr">
@@ -52438,6 +53438,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="6" t="inlineStr">
@@ -52472,6 +53477,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="6" t="inlineStr">
@@ -52506,6 +53516,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="6" t="inlineStr">
@@ -52540,6 +53555,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="6" t="inlineStr">
@@ -52574,6 +53594,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="6" t="inlineStr">
@@ -52608,6 +53633,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="6" t="inlineStr">
@@ -52642,6 +53672,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="6" t="inlineStr">
@@ -52676,6 +53711,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="6" t="inlineStr">
@@ -52710,6 +53750,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="6" t="inlineStr">
@@ -52744,6 +53789,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="6" t="inlineStr">
@@ -52778,6 +53828,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="6" t="inlineStr">
@@ -52812,6 +53867,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="6" t="inlineStr">
@@ -52846,6 +53906,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="6" t="inlineStr">
@@ -52880,6 +53945,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="6" t="inlineStr">
@@ -52914,6 +53984,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="6" t="inlineStr">
@@ -52948,6 +54023,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="6" t="inlineStr">
@@ -52982,6 +54062,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="6" t="inlineStr">
@@ -53016,6 +54101,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="6" t="inlineStr">
@@ -53050,6 +54140,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="6" t="inlineStr">
@@ -53084,6 +54179,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="6" t="inlineStr">
@@ -53118,6 +54218,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="6" t="inlineStr">
@@ -53152,6 +54257,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="6" t="inlineStr">
@@ -53186,6 +54296,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="6" t="inlineStr">
@@ -53220,6 +54335,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="6" t="inlineStr">
@@ -53254,6 +54374,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="6" t="inlineStr">
@@ -53288,6 +54413,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="6" t="inlineStr">
@@ -53322,6 +54452,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="6" t="inlineStr">
@@ -53356,6 +54491,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="6" t="inlineStr">
@@ -53390,6 +54530,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="6" t="inlineStr">
@@ -53424,6 +54569,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="6" t="inlineStr">
@@ -53458,6 +54608,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="6" t="inlineStr">
@@ -53492,6 +54647,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="6" t="inlineStr">
@@ -53526,6 +54686,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="6" t="inlineStr">
@@ -53560,6 +54725,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="6" t="inlineStr">
@@ -53594,6 +54764,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="6" t="inlineStr">
@@ -53628,6 +54803,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="6" t="inlineStr">
@@ -53662,6 +54842,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="6" t="inlineStr">
@@ -53696,6 +54881,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="6" t="inlineStr">
@@ -53730,6 +54920,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="6" t="inlineStr">
@@ -53764,6 +54959,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="6" t="inlineStr">
@@ -53798,6 +54998,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="6" t="inlineStr">
@@ -53832,6 +55037,11 @@
           <t>c__Clostridia</t>
         </is>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="6" t="inlineStr">
@@ -53866,6 +55076,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="6" t="inlineStr">
@@ -53896,6 +55111,11 @@
         </is>
       </c>
       <c r="H132" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
         <is>
           <t>reject</t>
         </is>
@@ -56620,7 +57840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56664,6 +57884,11 @@
           <t>rejection-0.98</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -56698,6 +57923,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -56732,6 +57962,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -56766,6 +58001,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -56800,6 +58040,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -56834,6 +58079,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -56868,6 +58118,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -56902,6 +58157,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -56936,6 +58196,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -56970,6 +58235,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -57004,6 +58274,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -57038,6 +58313,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -57072,6 +58352,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -57106,6 +58391,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -57140,6 +58430,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -57174,6 +58469,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -57208,6 +58508,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -57242,6 +58547,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -57276,6 +58586,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
@@ -57310,6 +58625,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
@@ -57344,6 +58664,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
@@ -57378,6 +58703,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
@@ -57412,6 +58742,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
@@ -57446,6 +58781,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
@@ -57480,6 +58820,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
@@ -57514,6 +58859,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
@@ -57548,6 +58898,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
@@ -57582,6 +58937,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
@@ -57616,6 +58976,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
@@ -57650,6 +59015,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
@@ -57684,6 +59054,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
@@ -57718,6 +59093,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
@@ -57752,6 +59132,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
@@ -57786,6 +59171,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
@@ -57820,6 +59210,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
@@ -57850,6 +59245,11 @@
         </is>
       </c>
       <c r="H36" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>reject</t>
         </is>
@@ -57866,7 +59266,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57910,6 +59310,11 @@
           <t>rejection-0.98</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -57944,6 +59349,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -57978,6 +59388,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -58012,6 +59427,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -58046,6 +59466,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -58080,6 +59505,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -58114,6 +59544,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -58148,6 +59583,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -58182,6 +59622,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -58216,6 +59661,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -58250,6 +59700,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -58284,6 +59739,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -58318,6 +59778,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -58352,6 +59817,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -58386,6 +59856,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -58420,6 +59895,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -58454,6 +59934,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -58488,6 +59973,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -58522,6 +60012,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
@@ -58556,6 +60051,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
@@ -58590,6 +60090,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
@@ -58624,6 +60129,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
@@ -58658,6 +60168,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
@@ -58692,6 +60207,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
@@ -58726,6 +60246,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
@@ -58760,6 +60285,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
@@ -58794,6 +60324,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
@@ -58828,6 +60363,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
@@ -58862,6 +60402,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
@@ -58896,6 +60441,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
@@ -58930,6 +60480,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
@@ -58964,6 +60519,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
@@ -58998,6 +60558,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
@@ -59032,6 +60597,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
@@ -59066,6 +60636,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
@@ -59100,6 +60675,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
@@ -59134,6 +60714,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
@@ -59168,6 +60753,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
@@ -59202,6 +60792,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
@@ -59236,6 +60831,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
@@ -59270,6 +60870,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
@@ -59304,6 +60909,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
@@ -59338,6 +60948,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
@@ -59372,6 +60987,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
@@ -59406,6 +61026,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
@@ -59440,6 +61065,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
@@ -59474,6 +61104,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
@@ -59508,6 +61143,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
@@ -59542,6 +61182,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>c__Clostridia</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
@@ -59576,6 +61221,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
@@ -59610,6 +61260,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
@@ -59644,6 +61299,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
@@ -59678,6 +61338,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="6" t="inlineStr">
@@ -59712,6 +61377,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
@@ -59746,6 +61416,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
@@ -59780,6 +61455,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
@@ -59814,6 +61494,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
@@ -59848,6 +61533,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
@@ -59882,6 +61572,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
@@ -59916,6 +61611,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
@@ -59950,6 +61650,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="6" t="inlineStr">
@@ -59984,6 +61689,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="6" t="inlineStr">
@@ -60018,6 +61728,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
@@ -60052,6 +61767,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
@@ -60086,6 +61806,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="6" t="inlineStr">
@@ -60120,6 +61845,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="6" t="inlineStr">
@@ -60154,6 +61884,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="6" t="inlineStr">
@@ -60188,6 +61923,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
@@ -60222,6 +61962,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="6" t="inlineStr">
@@ -60256,6 +62001,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="6" t="inlineStr">
@@ -60290,6 +62040,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="6" t="inlineStr">
@@ -60324,6 +62079,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="6" t="inlineStr">
@@ -60358,6 +62118,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="6" t="inlineStr">
@@ -60392,6 +62157,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="6" t="inlineStr">
@@ -60426,6 +62196,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="6" t="inlineStr">
@@ -60460,6 +62235,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="6" t="inlineStr">
@@ -60494,6 +62274,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="6" t="inlineStr">
@@ -60528,6 +62313,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="6" t="inlineStr">
@@ -60562,6 +62352,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="6" t="inlineStr">
@@ -60596,6 +62391,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="6" t="inlineStr">
@@ -60630,6 +62430,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="6" t="inlineStr">
@@ -60664,6 +62469,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="6" t="inlineStr">
@@ -60698,6 +62508,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="6" t="inlineStr">
@@ -60732,6 +62547,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="6" t="inlineStr">
@@ -60766,6 +62586,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="6" t="inlineStr">
@@ -60800,6 +62625,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="6" t="inlineStr">
@@ -60834,6 +62664,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="6" t="inlineStr">
@@ -60868,6 +62703,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="6" t="inlineStr">
@@ -60902,6 +62742,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="6" t="inlineStr">
@@ -60936,6 +62781,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="6" t="inlineStr">
@@ -60970,6 +62820,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="6" t="inlineStr">
@@ -61004,6 +62859,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="6" t="inlineStr">
@@ -61038,6 +62898,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="6" t="inlineStr">
@@ -61072,6 +62937,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="6" t="inlineStr">
@@ -61106,6 +62976,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="6" t="inlineStr">
@@ -61140,6 +63015,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="6" t="inlineStr">
@@ -61174,6 +63054,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="6" t="inlineStr">
@@ -61208,6 +63093,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="6" t="inlineStr">
@@ -61242,6 +63132,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="6" t="inlineStr">
@@ -61276,6 +63171,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="6" t="inlineStr">
@@ -61310,6 +63210,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="6" t="inlineStr">
@@ -61344,6 +63249,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="6" t="inlineStr">
@@ -61378,6 +63288,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="6" t="inlineStr">
@@ -61412,6 +63327,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="6" t="inlineStr">
@@ -61446,6 +63366,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="6" t="inlineStr">
@@ -61480,6 +63405,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="6" t="inlineStr">
@@ -61514,6 +63444,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="6" t="inlineStr">
@@ -61548,6 +63483,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="6" t="inlineStr">
@@ -61582,6 +63522,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="6" t="inlineStr">
@@ -61616,6 +63561,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="6" t="inlineStr">
@@ -61650,6 +63600,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="6" t="inlineStr">
@@ -61684,6 +63639,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="6" t="inlineStr">
@@ -61718,6 +63678,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="6" t="inlineStr">
@@ -61752,6 +63717,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="6" t="inlineStr">
@@ -61786,6 +63756,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="6" t="inlineStr">
@@ -61820,6 +63795,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="6" t="inlineStr">
@@ -61854,6 +63834,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="6" t="inlineStr">
@@ -61888,6 +63873,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="6" t="inlineStr">
@@ -61922,6 +63912,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="6" t="inlineStr">
@@ -61956,6 +63951,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="6" t="inlineStr">
@@ -61990,6 +63990,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="6" t="inlineStr">
@@ -62024,6 +64029,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="6" t="inlineStr">
@@ -62058,6 +64068,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="6" t="inlineStr">
@@ -62092,6 +64107,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="6" t="inlineStr">
@@ -62126,6 +64146,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="6" t="inlineStr">
@@ -62160,6 +64185,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="6" t="inlineStr">
@@ -62194,6 +64224,11 @@
           <t>reject</t>
         </is>
       </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="6" t="inlineStr">
@@ -62224,6 +64259,11 @@
         </is>
       </c>
       <c r="H128" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
         <is>
           <t>reject</t>
         </is>

</xml_diff>